<commit_message>
Write type to spreadsheet
</commit_message>
<xml_diff>
--- a/Crawl_with_Class.xlsx
+++ b/Crawl_with_Class.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="456">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="458">
   <si>
     <t>AD = Andorra</t>
   </si>
@@ -608,6 +608,9 @@
     <t>HT = Haiti</t>
   </si>
   <si>
+    <t>HTTP</t>
+  </si>
+  <si>
     <t>HU = Hungary</t>
   </si>
   <si>
@@ -963,6 +966,9 @@
   </si>
   <si>
     <t>Nigerian  Academy of Sciences</t>
+  </si>
+  <si>
+    <t>None</t>
   </si>
   <si>
     <t>Norwegian Academy of Sciences and  Letters</t>
@@ -1738,100 +1744,124 @@
   <sheetFormatPr defaultRowHeight="15" baseColWidth="10"/>
   <sheetData>
     <row spans="1:9" r="1">
-      <c r="A1" s="1" t="s">
-        <v>413</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>252</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>419</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>319</v>
-      </c>
-      <c r="E1" s="1" t="s">
+      <c t="s" s="1" r="A1">
+        <v>415</v>
+      </c>
+      <c t="s" s="1" r="B1">
+        <v>253</v>
+      </c>
+      <c t="s" s="1" r="C1">
+        <v>421</v>
+      </c>
+      <c t="s" s="1" r="D1">
+        <v>321</v>
+      </c>
+      <c t="s" s="1" r="E1">
         <v>137</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>343</v>
-      </c>
-      <c r="G1" s="1" t="s">
+      <c t="s" s="1" r="F1">
+        <v>345</v>
+      </c>
+      <c t="s" s="1" r="G1">
         <v>126</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>401</v>
-      </c>
-      <c r="I1" s="1" t="s">
+      <c t="s" s="1" r="H1">
+        <v>403</v>
+      </c>
+      <c t="s" s="1" r="I1">
         <v>127</v>
       </c>
     </row>
     <row spans="1:9" r="2">
-      <c r="A2" t="s">
+      <c t="s" r="A2">
         <v>99</v>
       </c>
-      <c r="C2" t="s">
-        <v>449</v>
+      <c t="s" r="C2">
+        <v>451</v>
+      </c>
+      <c t="s" r="G2">
+        <v>316</v>
       </c>
     </row>
     <row spans="1:9" r="3">
-      <c r="A3" t="s">
+      <c t="s" r="A3">
         <v>100</v>
       </c>
-      <c r="C3" t="s">
-        <v>450</v>
+      <c t="s" r="C3">
+        <v>452</v>
+      </c>
+      <c t="s" r="G3">
+        <v>196</v>
       </c>
     </row>
     <row spans="1:9" r="4">
-      <c r="A4" t="s">
+      <c t="s" r="A4">
         <v>101</v>
       </c>
-      <c r="C4" t="s">
-        <v>451</v>
+      <c t="s" r="C4">
+        <v>453</v>
+      </c>
+      <c t="s" r="G4">
+        <v>196</v>
       </c>
     </row>
     <row spans="1:9" r="5">
-      <c r="A5" t="s">
+      <c t="s" r="A5">
         <v>190</v>
       </c>
-      <c r="C5" t="s">
-        <v>452</v>
+      <c t="s" r="C5">
+        <v>454</v>
+      </c>
+      <c t="s" r="G5">
+        <v>196</v>
       </c>
     </row>
     <row spans="1:9" r="6">
-      <c r="A6" t="s">
-        <v>378</v>
-      </c>
-      <c r="C6" t="s">
-        <v>453</v>
+      <c t="s" r="A6">
+        <v>380</v>
+      </c>
+      <c t="s" r="C6">
+        <v>455</v>
+      </c>
+      <c t="s" r="G6">
+        <v>196</v>
       </c>
     </row>
     <row spans="1:9" r="7">
-      <c r="A7" t="s">
+      <c t="s" r="A7">
         <v>163</v>
       </c>
-      <c r="C7" t="s">
-        <v>454</v>
+      <c t="s" r="C7">
+        <v>456</v>
+      </c>
+      <c t="s" r="G7">
+        <v>196</v>
       </c>
     </row>
     <row spans="1:9" r="8">
-      <c r="A8" t="s">
+      <c t="s" r="A8">
         <v>163</v>
       </c>
-      <c r="C8" t="s">
-        <v>454</v>
+      <c t="s" r="C8">
+        <v>456</v>
+      </c>
+      <c t="s" r="G8">
+        <v>196</v>
       </c>
     </row>
     <row spans="1:9" r="9">
-      <c r="A9" t="s">
+      <c t="s" r="A9">
         <v>163</v>
       </c>
-      <c r="C9" t="s">
-        <v>454</v>
+      <c t="s" r="C9">
+        <v>456</v>
+      </c>
+      <c t="s" r="G9">
+        <v>196</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins top="1" footer="0.5" right="0.75" header="0.5" left="0.75" bottom="1"/>
+  <pageMargins bottom="1" right="0.75" left="0.75" top="1" footer="0.5" header="0.5"/>
 </worksheet>
 </file>
 
@@ -1849,36 +1879,36 @@
   <sheetFormatPr defaultRowHeight="15" baseColWidth="10"/>
   <sheetData>
     <row spans="1:9" r="1">
-      <c r="A1" s="1" t="s">
-        <v>413</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>252</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>419</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>319</v>
-      </c>
-      <c r="E1" s="1" t="s">
+      <c t="s" s="1" r="A1">
+        <v>415</v>
+      </c>
+      <c t="s" s="1" r="B1">
+        <v>253</v>
+      </c>
+      <c t="s" s="1" r="C1">
+        <v>421</v>
+      </c>
+      <c t="s" s="1" r="D1">
+        <v>321</v>
+      </c>
+      <c t="s" s="1" r="E1">
         <v>137</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>343</v>
-      </c>
-      <c r="G1" s="1" t="s">
+      <c t="s" s="1" r="F1">
+        <v>345</v>
+      </c>
+      <c t="s" s="1" r="G1">
         <v>126</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>401</v>
-      </c>
-      <c r="I1" s="1" t="s">
+      <c t="s" s="1" r="H1">
+        <v>403</v>
+      </c>
+      <c t="s" s="1" r="I1">
         <v>127</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins top="1" footer="0.5" right="0.75" header="0.5" left="0.75" bottom="1"/>
+  <pageMargins bottom="1" right="0.75" left="0.75" top="1" footer="0.5" header="0.5"/>
 </worksheet>
 </file>
 
@@ -1896,917 +1926,917 @@
   <sheetFormatPr defaultRowHeight="15" baseColWidth="10"/>
   <sheetData>
     <row spans="1:1" r="2">
-      <c r="A2" t="s">
+      <c t="s" r="A2">
         <v>17</v>
       </c>
     </row>
     <row spans="1:1" r="3">
-      <c r="A3" t="s">
+      <c t="s" r="A3">
         <v>21</v>
       </c>
     </row>
     <row spans="1:1" r="4">
-      <c r="A4" t="s">
+      <c t="s" r="A4">
         <v>23</v>
       </c>
     </row>
     <row spans="1:1" r="5">
-      <c r="A5" t="s">
+      <c t="s" r="A5">
         <v>22</v>
       </c>
     </row>
     <row spans="1:1" r="6">
-      <c r="A6" t="s">
+      <c t="s" r="A6">
         <v>18</v>
       </c>
     </row>
     <row spans="1:1" r="7">
-      <c r="A7" t="s">
+      <c t="s" r="A7">
         <v>19</v>
       </c>
     </row>
     <row spans="1:1" r="8">
-      <c r="A8" t="s">
+      <c t="s" r="A8">
         <v>20</v>
       </c>
     </row>
     <row spans="1:1" r="9">
-      <c r="A9" t="s">
+      <c t="s" r="A9">
         <v>34</v>
       </c>
     </row>
     <row spans="1:1" r="10">
-      <c r="A10" t="s">
+      <c t="s" r="A10">
         <v>35</v>
       </c>
     </row>
     <row spans="1:1" r="11">
-      <c r="A11" t="s">
+      <c t="s" r="A11">
         <v>24</v>
       </c>
     </row>
     <row spans="1:1" r="12">
-      <c r="A12" t="s">
+      <c t="s" r="A12">
         <v>31</v>
       </c>
     </row>
     <row spans="1:1" r="13">
-      <c r="A13" t="s">
+      <c t="s" r="A13">
         <v>25</v>
       </c>
     </row>
     <row spans="1:1" r="14">
-      <c r="A14" t="s">
+      <c t="s" r="A14">
         <v>26</v>
       </c>
     </row>
     <row spans="1:1" r="15">
-      <c r="A15" t="s">
+      <c t="s" r="A15">
         <v>33</v>
       </c>
     </row>
     <row spans="1:1" r="16">
-      <c r="A16" t="s">
+      <c t="s" r="A16">
         <v>32</v>
       </c>
     </row>
     <row spans="1:1" r="17">
-      <c r="A17" t="s">
+      <c t="s" r="A17">
         <v>27</v>
       </c>
     </row>
     <row spans="1:1" r="18">
-      <c r="A18" t="s">
+      <c t="s" r="A18">
         <v>28</v>
       </c>
     </row>
     <row spans="1:1" r="19">
-      <c r="A19" t="s">
+      <c t="s" r="A19">
         <v>29</v>
       </c>
     </row>
     <row spans="1:1" r="20">
-      <c r="A20" t="s">
+      <c t="s" r="A20">
         <v>30</v>
       </c>
     </row>
     <row spans="1:1" r="21">
-      <c r="A21" t="s">
+      <c t="s" r="A21">
         <v>36</v>
       </c>
     </row>
     <row spans="1:1" r="22">
-      <c r="A22" t="s">
+      <c t="s" r="A22">
         <v>37</v>
       </c>
     </row>
     <row spans="1:1" r="23">
-      <c r="A23" t="s">
+      <c t="s" r="A23">
         <v>38</v>
       </c>
     </row>
     <row spans="1:1" r="24">
-      <c r="A24" t="s">
+      <c t="s" r="A24">
         <v>39</v>
       </c>
     </row>
     <row spans="1:1" r="25">
-      <c r="A25" t="s">
+      <c t="s" r="A25">
         <v>40</v>
       </c>
     </row>
     <row spans="1:1" r="26">
-      <c r="A26" t="s">
+      <c t="s" r="A26">
         <v>41</v>
       </c>
     </row>
     <row spans="1:1" r="27">
-      <c r="A27" t="s">
+      <c t="s" r="A27">
         <v>42</v>
       </c>
     </row>
     <row spans="1:1" r="28">
-      <c r="A28" t="s">
+      <c t="s" r="A28">
         <v>53</v>
       </c>
     </row>
     <row spans="1:1" r="29">
-      <c r="A29" t="s">
+      <c t="s" r="A29">
         <v>43</v>
       </c>
     </row>
     <row spans="1:1" r="30">
-      <c r="A30" t="s">
+      <c t="s" r="A30">
         <v>44</v>
       </c>
     </row>
     <row spans="1:1" r="31">
-      <c r="A31" t="s">
+      <c t="s" r="A31">
         <v>54</v>
       </c>
     </row>
     <row spans="1:1" r="32">
-      <c r="A32" t="s">
+      <c t="s" r="A32">
         <v>45</v>
       </c>
     </row>
     <row spans="1:1" r="33">
-      <c r="A33" t="s">
+      <c t="s" r="A33">
         <v>46</v>
       </c>
     </row>
     <row spans="1:1" r="34">
-      <c r="A34" t="s">
+      <c t="s" r="A34">
         <v>55</v>
       </c>
     </row>
     <row spans="1:1" r="35">
-      <c r="A35" t="s">
+      <c t="s" r="A35">
         <v>56</v>
       </c>
     </row>
     <row spans="1:1" r="36">
-      <c r="A36" t="s">
+      <c t="s" r="A36">
         <v>47</v>
       </c>
     </row>
     <row spans="1:1" r="37">
-      <c r="A37" t="s">
+      <c t="s" r="A37">
         <v>57</v>
       </c>
     </row>
     <row spans="1:1" r="38">
-      <c r="A38" t="s">
+      <c t="s" r="A38">
         <v>58</v>
       </c>
     </row>
     <row spans="1:1" r="39">
-      <c r="A39" t="s">
+      <c t="s" r="A39">
         <v>48</v>
       </c>
     </row>
     <row spans="1:1" r="40">
-      <c r="A40" t="s">
+      <c t="s" r="A40">
         <v>59</v>
       </c>
     </row>
     <row spans="1:1" r="41">
-      <c r="A41" t="s">
+      <c t="s" r="A41">
         <v>49</v>
       </c>
     </row>
     <row spans="1:1" r="42">
-      <c r="A42" t="s">
+      <c t="s" r="A42">
         <v>50</v>
       </c>
     </row>
     <row spans="1:1" r="43">
-      <c r="A43" t="s">
+      <c t="s" r="A43">
         <v>51</v>
       </c>
     </row>
     <row spans="1:1" r="44">
-      <c r="A44" t="s">
+      <c t="s" r="A44">
         <v>52</v>
       </c>
     </row>
     <row spans="1:1" r="45">
-      <c r="A45" t="s">
+      <c t="s" r="A45">
         <v>60</v>
       </c>
     </row>
     <row spans="1:1" r="46">
-      <c r="A46" t="s">
+      <c t="s" r="A46">
         <v>61</v>
       </c>
     </row>
     <row spans="1:1" r="47">
-      <c r="A47" t="s">
+      <c t="s" r="A47">
         <v>62</v>
       </c>
     </row>
     <row spans="1:1" r="48">
-      <c r="A48" t="s">
+      <c t="s" r="A48">
         <v>67</v>
       </c>
     </row>
     <row spans="1:1" r="49">
-      <c r="A49" t="s">
+      <c t="s" r="A49">
         <v>63</v>
       </c>
     </row>
     <row spans="1:1" r="50">
-      <c r="A50" t="s">
+      <c t="s" r="A50">
         <v>64</v>
       </c>
     </row>
     <row spans="1:1" r="51">
-      <c r="A51" t="s">
+      <c t="s" r="A51">
         <v>65</v>
       </c>
     </row>
     <row spans="1:1" r="52">
-      <c r="A52" t="s">
+      <c t="s" r="A52">
         <v>66</v>
       </c>
     </row>
     <row spans="1:1" r="53">
-      <c r="A53" t="s">
+      <c t="s" r="A53">
         <v>68</v>
       </c>
     </row>
     <row spans="1:1" r="54">
-      <c r="A54" t="s">
+      <c t="s" r="A54">
         <v>88</v>
       </c>
     </row>
     <row spans="1:1" r="55">
-      <c r="A55" t="s">
+      <c t="s" r="A55">
         <v>89</v>
       </c>
     </row>
     <row spans="1:1" r="56">
-      <c r="A56" t="s">
+      <c t="s" r="A56">
         <v>90</v>
       </c>
     </row>
     <row spans="1:1" r="57">
-      <c r="A57" t="s">
+      <c t="s" r="A57">
         <v>91</v>
       </c>
     </row>
     <row spans="1:1" r="58">
-      <c r="A58" t="s">
+      <c t="s" r="A58">
         <v>92</v>
       </c>
     </row>
     <row spans="1:1" r="59">
-      <c r="A59" t="s">
+      <c t="s" r="A59">
         <v>115</v>
       </c>
     </row>
     <row spans="1:1" r="60">
-      <c r="A60" t="s">
+      <c t="s" r="A60">
         <v>116</v>
       </c>
     </row>
     <row spans="1:1" r="61">
-      <c r="A61" t="s">
+      <c t="s" r="A61">
         <v>120</v>
       </c>
     </row>
     <row spans="1:1" r="62">
-      <c r="A62" t="s">
+      <c t="s" r="A62">
         <v>117</v>
       </c>
     </row>
     <row spans="1:1" r="63">
-      <c r="A63" t="s">
+      <c t="s" r="A63">
         <v>121</v>
       </c>
     </row>
     <row spans="1:1" r="64">
-      <c r="A64" t="s">
+      <c t="s" r="A64">
         <v>118</v>
       </c>
     </row>
     <row spans="1:1" r="65">
-      <c r="A65" t="s">
+      <c t="s" r="A65">
         <v>119</v>
       </c>
     </row>
     <row spans="1:1" r="66">
-      <c r="A66" t="s">
+      <c t="s" r="A66">
         <v>122</v>
       </c>
     </row>
     <row spans="1:1" r="67">
-      <c r="A67" t="s">
+      <c t="s" r="A67">
         <v>123</v>
       </c>
     </row>
     <row spans="1:1" r="68">
-      <c r="A68" t="s">
+      <c t="s" r="A68">
         <v>124</v>
       </c>
     </row>
     <row spans="1:1" r="69">
-      <c r="A69" t="s">
+      <c t="s" r="A69">
         <v>125</v>
       </c>
     </row>
     <row spans="1:1" r="70">
-      <c r="A70" t="s">
+      <c t="s" r="A70">
         <v>128</v>
       </c>
     </row>
     <row spans="1:1" r="71">
-      <c r="A71" t="s">
+      <c t="s" r="A71">
         <v>129</v>
       </c>
     </row>
     <row spans="1:1" r="72">
-      <c r="A72" t="s">
+      <c t="s" r="A72">
         <v>136</v>
       </c>
     </row>
     <row spans="1:1" r="73">
-      <c r="A73" t="s">
+      <c t="s" r="A73">
         <v>148</v>
       </c>
     </row>
     <row spans="1:1" r="74">
-      <c r="A74" t="s">
+      <c t="s" r="A74">
         <v>147</v>
       </c>
     </row>
     <row spans="1:1" r="75">
-      <c r="A75" t="s">
+      <c t="s" r="A75">
         <v>149</v>
       </c>
     </row>
     <row spans="1:1" r="76">
-      <c r="A76" t="s">
+      <c t="s" r="A76">
         <v>153</v>
       </c>
     </row>
     <row spans="1:1" r="77">
-      <c r="A77" t="s">
+      <c t="s" r="A77">
         <v>154</v>
       </c>
     </row>
     <row spans="1:1" r="78">
-      <c r="A78" t="s">
+      <c t="s" r="A78">
         <v>150</v>
       </c>
     </row>
     <row spans="1:1" r="79">
-      <c r="A79" t="s">
+      <c t="s" r="A79">
         <v>151</v>
       </c>
     </row>
     <row spans="1:1" r="80">
-      <c r="A80" t="s">
+      <c t="s" r="A80">
         <v>152</v>
       </c>
     </row>
     <row spans="1:1" r="81">
-      <c r="A81" t="s">
+      <c t="s" r="A81">
         <v>162</v>
       </c>
     </row>
     <row spans="1:1" r="82">
-      <c r="A82" t="s">
+      <c t="s" r="A82">
         <v>164</v>
       </c>
     </row>
     <row spans="1:1" r="83">
-      <c r="A83" t="s">
+      <c t="s" r="A83">
         <v>184</v>
       </c>
     </row>
     <row spans="1:1" r="84">
-      <c r="A84" t="s">
+      <c t="s" r="A84">
         <v>185</v>
       </c>
     </row>
     <row spans="1:1" r="85">
-      <c r="A85" t="s">
+      <c t="s" r="A85">
         <v>186</v>
       </c>
     </row>
     <row spans="1:1" r="86">
-      <c r="A86" t="s">
+      <c t="s" r="A86">
         <v>187</v>
       </c>
     </row>
     <row spans="1:1" r="87">
-      <c r="A87" t="s">
+      <c t="s" r="A87">
         <v>188</v>
       </c>
     </row>
     <row spans="1:1" r="88">
-      <c r="A88" t="s">
+      <c t="s" r="A88">
         <v>189</v>
       </c>
     </row>
     <row spans="1:1" r="89">
-      <c r="A89" t="s">
-        <v>207</v>
+      <c t="s" r="A89">
+        <v>208</v>
       </c>
     </row>
     <row spans="1:1" r="90">
-      <c r="A90" t="s">
-        <v>208</v>
+      <c t="s" r="A90">
+        <v>209</v>
       </c>
     </row>
     <row spans="1:1" r="91">
-      <c r="A91" t="s">
-        <v>209</v>
+      <c t="s" r="A91">
+        <v>210</v>
       </c>
     </row>
     <row spans="1:1" r="92">
-      <c r="A92" t="s">
-        <v>210</v>
+      <c t="s" r="A92">
+        <v>211</v>
       </c>
     </row>
     <row spans="1:1" r="93">
-      <c r="A93" t="s">
-        <v>211</v>
+      <c t="s" r="A93">
+        <v>212</v>
       </c>
     </row>
     <row spans="1:1" r="94">
-      <c r="A94" t="s">
-        <v>212</v>
+      <c t="s" r="A94">
+        <v>213</v>
       </c>
     </row>
     <row spans="1:1" r="95">
-      <c r="A95" t="s">
+      <c t="s" r="A95">
+        <v>215</v>
+      </c>
+    </row>
+    <row spans="1:1" r="96">
+      <c t="s" r="A96">
+        <v>216</v>
+      </c>
+    </row>
+    <row spans="1:1" r="97">
+      <c t="s" r="A97">
+        <v>217</v>
+      </c>
+    </row>
+    <row spans="1:1" r="98">
+      <c t="s" r="A98">
+        <v>218</v>
+      </c>
+    </row>
+    <row spans="1:1" r="99">
+      <c t="s" r="A99">
+        <v>219</v>
+      </c>
+    </row>
+    <row spans="1:1" r="100">
+      <c t="s" r="A100">
         <v>214</v>
       </c>
     </row>
-    <row spans="1:1" r="96">
-      <c r="A96" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row spans="1:1" r="97">
-      <c r="A97" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row spans="1:1" r="98">
-      <c r="A98" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row spans="1:1" r="99">
-      <c r="A99" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row spans="1:1" r="100">
-      <c r="A100" t="s">
-        <v>213</v>
-      </c>
-    </row>
     <row spans="1:1" r="101">
-      <c r="A101" t="s">
-        <v>219</v>
+      <c t="s" r="A101">
+        <v>220</v>
       </c>
     </row>
     <row spans="1:1" r="102">
-      <c r="A102" t="s">
-        <v>220</v>
+      <c t="s" r="A102">
+        <v>221</v>
       </c>
     </row>
     <row spans="1:1" r="103">
-      <c r="A103" t="s">
-        <v>221</v>
+      <c t="s" r="A103">
+        <v>222</v>
       </c>
     </row>
     <row spans="1:1" r="104">
-      <c r="A104" t="s">
-        <v>222</v>
+      <c t="s" r="A104">
+        <v>223</v>
       </c>
     </row>
     <row spans="1:1" r="105">
-      <c r="A105" t="s">
-        <v>223</v>
+      <c t="s" r="A105">
+        <v>224</v>
       </c>
     </row>
     <row spans="1:1" r="106">
-      <c r="A106" t="s">
-        <v>238</v>
+      <c t="s" r="A106">
+        <v>239</v>
       </c>
     </row>
     <row spans="1:1" r="107">
-      <c r="A107" t="s">
-        <v>239</v>
+      <c t="s" r="A107">
+        <v>240</v>
       </c>
     </row>
     <row spans="1:1" r="108">
-      <c r="A108" t="s">
-        <v>240</v>
+      <c t="s" r="A108">
+        <v>241</v>
       </c>
     </row>
     <row spans="1:1" r="109">
-      <c r="A109" t="s">
-        <v>455</v>
+      <c t="s" r="A109">
+        <v>457</v>
       </c>
     </row>
     <row spans="1:1" r="110">
-      <c r="A110" t="s">
-        <v>253</v>
+      <c t="s" r="A110">
+        <v>254</v>
       </c>
     </row>
     <row spans="1:1" r="111">
-      <c r="A111" t="s">
-        <v>254</v>
+      <c t="s" r="A111">
+        <v>255</v>
       </c>
     </row>
     <row spans="1:1" r="112">
-      <c r="A112" t="s">
-        <v>255</v>
+      <c t="s" r="A112">
+        <v>256</v>
       </c>
     </row>
     <row spans="1:1" r="113">
-      <c r="A113" t="s">
-        <v>278</v>
+      <c t="s" r="A113">
+        <v>279</v>
       </c>
     </row>
     <row spans="1:1" r="114">
-      <c r="A114" t="s">
+      <c t="s" r="A114">
+        <v>299</v>
+      </c>
+    </row>
+    <row spans="1:1" r="115">
+      <c t="s" r="A115">
+        <v>301</v>
+      </c>
+    </row>
+    <row spans="1:1" r="116">
+      <c t="s" r="A116">
+        <v>300</v>
+      </c>
+    </row>
+    <row spans="1:1" r="117">
+      <c t="s" r="A117">
+        <v>302</v>
+      </c>
+    </row>
+    <row spans="1:1" r="118">
+      <c t="s" r="A118">
+        <v>303</v>
+      </c>
+    </row>
+    <row spans="1:1" r="119">
+      <c t="s" r="A119">
+        <v>304</v>
+      </c>
+    </row>
+    <row spans="1:1" r="120">
+      <c t="s" r="A120">
+        <v>306</v>
+      </c>
+    </row>
+    <row spans="1:1" r="121">
+      <c t="s" r="A121">
+        <v>305</v>
+      </c>
+    </row>
+    <row spans="1:1" r="122">
+      <c t="s" r="A122">
+        <v>295</v>
+      </c>
+    </row>
+    <row spans="1:1" r="123">
+      <c t="s" r="A123">
+        <v>296</v>
+      </c>
+    </row>
+    <row spans="1:1" r="124">
+      <c t="s" r="A124">
+        <v>307</v>
+      </c>
+    </row>
+    <row spans="1:1" r="125">
+      <c t="s" r="A125">
+        <v>308</v>
+      </c>
+    </row>
+    <row spans="1:1" r="126">
+      <c t="s" r="A126">
+        <v>297</v>
+      </c>
+    </row>
+    <row spans="1:1" r="127">
+      <c t="s" r="A127">
         <v>298</v>
       </c>
     </row>
-    <row spans="1:1" r="115">
-      <c r="A115" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row spans="1:1" r="116">
-      <c r="A116" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row spans="1:1" r="117">
-      <c r="A117" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row spans="1:1" r="118">
-      <c r="A118" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row spans="1:1" r="119">
-      <c r="A119" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row spans="1:1" r="120">
-      <c r="A120" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row spans="1:1" r="121">
-      <c r="A121" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row spans="1:1" r="122">
-      <c r="A122" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row spans="1:1" r="123">
-      <c r="A123" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row spans="1:1" r="124">
-      <c r="A124" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row spans="1:1" r="125">
-      <c r="A125" t="s">
-        <v>307</v>
-      </c>
-    </row>
-    <row spans="1:1" r="126">
-      <c r="A126" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row spans="1:1" r="127">
-      <c r="A127" t="s">
-        <v>297</v>
-      </c>
-    </row>
     <row spans="1:1" r="128">
-      <c r="A128" t="s">
+      <c t="s" r="A128">
+        <v>310</v>
+      </c>
+    </row>
+    <row spans="1:1" r="129">
+      <c t="s" r="A129">
+        <v>311</v>
+      </c>
+    </row>
+    <row spans="1:1" r="130">
+      <c t="s" r="A130">
         <v>309</v>
       </c>
     </row>
-    <row spans="1:1" r="129">
-      <c r="A129" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row spans="1:1" r="130">
-      <c r="A130" t="s">
-        <v>308</v>
-      </c>
-    </row>
     <row spans="1:1" r="131">
-      <c r="A131" t="s">
-        <v>311</v>
+      <c t="s" r="A131">
+        <v>312</v>
       </c>
     </row>
     <row spans="1:1" r="132">
-      <c r="A132" t="s">
-        <v>312</v>
+      <c t="s" r="A132">
+        <v>313</v>
       </c>
     </row>
     <row spans="1:1" r="133">
-      <c r="A133" t="s">
-        <v>313</v>
+      <c t="s" r="A133">
+        <v>314</v>
       </c>
     </row>
     <row spans="1:1" r="134">
-      <c r="A134" t="s">
-        <v>314</v>
+      <c t="s" r="A134">
+        <v>315</v>
       </c>
     </row>
     <row spans="1:1" r="135">
-      <c r="A135" t="s">
-        <v>315</v>
+      <c t="s" r="A135">
+        <v>317</v>
       </c>
     </row>
     <row spans="1:1" r="136">
-      <c r="A136" t="s">
-        <v>318</v>
+      <c t="s" r="A136">
+        <v>320</v>
       </c>
     </row>
     <row spans="1:1" r="137">
-      <c r="A137" t="s">
-        <v>320</v>
+      <c t="s" r="A137">
+        <v>322</v>
       </c>
     </row>
     <row spans="1:1" r="138">
-      <c r="A138" t="s">
-        <v>334</v>
+      <c t="s" r="A138">
+        <v>336</v>
       </c>
     </row>
     <row spans="1:1" r="139">
-      <c r="A139" t="s">
-        <v>335</v>
+      <c t="s" r="A139">
+        <v>337</v>
       </c>
     </row>
     <row spans="1:1" r="140">
-      <c r="A140" t="s">
-        <v>336</v>
+      <c t="s" r="A140">
+        <v>338</v>
       </c>
     </row>
     <row spans="1:1" r="141">
-      <c r="A141" t="s">
-        <v>337</v>
+      <c t="s" r="A141">
+        <v>339</v>
       </c>
     </row>
     <row spans="1:1" r="142">
-      <c r="A142" t="s">
-        <v>344</v>
+      <c t="s" r="A142">
+        <v>346</v>
       </c>
     </row>
     <row spans="1:1" r="143">
-      <c r="A143" t="s">
+      <c t="s" r="A143">
+        <v>350</v>
+      </c>
+    </row>
+    <row spans="1:1" r="144">
+      <c t="s" r="A144">
+        <v>351</v>
+      </c>
+    </row>
+    <row spans="1:1" r="145">
+      <c t="s" r="A145">
+        <v>352</v>
+      </c>
+    </row>
+    <row spans="1:1" r="146">
+      <c t="s" r="A146">
+        <v>347</v>
+      </c>
+    </row>
+    <row spans="1:1" r="147">
+      <c t="s" r="A147">
         <v>348</v>
       </c>
     </row>
-    <row spans="1:1" r="144">
-      <c r="A144" t="s">
+    <row spans="1:1" r="148">
+      <c t="s" r="A148">
+        <v>353</v>
+      </c>
+    </row>
+    <row spans="1:1" r="149">
+      <c t="s" r="A149">
         <v>349</v>
       </c>
     </row>
-    <row spans="1:1" r="145">
-      <c r="A145" t="s">
-        <v>350</v>
-      </c>
-    </row>
-    <row spans="1:1" r="146">
-      <c r="A146" t="s">
-        <v>345</v>
-      </c>
-    </row>
-    <row spans="1:1" r="147">
-      <c r="A147" t="s">
-        <v>346</v>
-      </c>
-    </row>
-    <row spans="1:1" r="148">
-      <c r="A148" t="s">
-        <v>351</v>
-      </c>
-    </row>
-    <row spans="1:1" r="149">
-      <c r="A149" t="s">
-        <v>347</v>
-      </c>
-    </row>
     <row spans="1:1" r="150">
-      <c r="A150" t="s">
-        <v>352</v>
+      <c t="s" r="A150">
+        <v>354</v>
       </c>
     </row>
     <row spans="1:1" r="151">
-      <c r="A151" t="s">
-        <v>353</v>
+      <c t="s" r="A151">
+        <v>355</v>
       </c>
     </row>
     <row spans="1:1" r="152">
-      <c r="A152" t="s">
-        <v>354</v>
+      <c t="s" r="A152">
+        <v>356</v>
       </c>
     </row>
     <row spans="1:1" r="153">
-      <c r="A153" t="s">
-        <v>355</v>
+      <c t="s" r="A153">
+        <v>357</v>
       </c>
     </row>
     <row spans="1:1" r="154">
-      <c r="A154" t="s">
-        <v>356</v>
+      <c t="s" r="A154">
+        <v>358</v>
       </c>
     </row>
     <row spans="1:1" r="155">
-      <c r="A155" t="s">
-        <v>357</v>
+      <c t="s" r="A155">
+        <v>359</v>
       </c>
     </row>
     <row spans="1:1" r="156">
-      <c r="A156" t="s">
-        <v>358</v>
+      <c t="s" r="A156">
+        <v>360</v>
       </c>
     </row>
     <row spans="1:1" r="157">
-      <c r="A157" t="s">
-        <v>381</v>
+      <c t="s" r="A157">
+        <v>383</v>
       </c>
     </row>
     <row spans="1:1" r="158">
-      <c r="A158" t="s">
-        <v>380</v>
+      <c t="s" r="A158">
+        <v>382</v>
       </c>
     </row>
     <row spans="1:1" r="159">
-      <c r="A159" t="s">
-        <v>383</v>
+      <c t="s" r="A159">
+        <v>385</v>
       </c>
     </row>
     <row spans="1:1" r="160">
-      <c r="A160" t="s">
-        <v>382</v>
+      <c t="s" r="A160">
+        <v>384</v>
       </c>
     </row>
     <row spans="1:1" r="161">
-      <c r="A161" t="s">
-        <v>384</v>
+      <c t="s" r="A161">
+        <v>386</v>
       </c>
     </row>
     <row spans="1:1" r="162">
-      <c r="A162" t="s">
-        <v>385</v>
+      <c t="s" r="A162">
+        <v>387</v>
       </c>
     </row>
     <row spans="1:1" r="163">
-      <c r="A163" t="s">
-        <v>386</v>
+      <c t="s" r="A163">
+        <v>388</v>
       </c>
     </row>
     <row spans="1:1" r="164">
-      <c r="A164" t="s">
-        <v>387</v>
+      <c t="s" r="A164">
+        <v>389</v>
       </c>
     </row>
     <row spans="1:1" r="165">
-      <c r="A165" t="s">
+      <c t="s" r="A165">
+        <v>392</v>
+      </c>
+    </row>
+    <row spans="1:1" r="166">
+      <c t="s" r="A166">
+        <v>393</v>
+      </c>
+    </row>
+    <row spans="1:1" r="167">
+      <c t="s" r="A167">
         <v>390</v>
       </c>
     </row>
-    <row spans="1:1" r="166">
-      <c r="A166" t="s">
+    <row spans="1:1" r="168">
+      <c t="s" r="A168">
         <v>391</v>
       </c>
     </row>
-    <row spans="1:1" r="167">
-      <c r="A167" t="s">
-        <v>388</v>
-      </c>
-    </row>
-    <row spans="1:1" r="168">
-      <c r="A168" t="s">
-        <v>389</v>
-      </c>
-    </row>
     <row spans="1:1" r="169">
-      <c r="A169" t="s">
-        <v>392</v>
+      <c t="s" r="A169">
+        <v>394</v>
       </c>
     </row>
     <row spans="1:1" r="170">
-      <c r="A170" t="s">
-        <v>393</v>
+      <c t="s" r="A170">
+        <v>395</v>
       </c>
     </row>
     <row spans="1:1" r="171">
-      <c r="A171" t="s">
-        <v>411</v>
+      <c t="s" r="A171">
+        <v>413</v>
       </c>
     </row>
     <row spans="1:1" r="172">
-      <c r="A172" t="s">
-        <v>412</v>
+      <c t="s" r="A172">
+        <v>414</v>
       </c>
     </row>
     <row spans="1:1" r="173">
-      <c r="A173" t="s">
-        <v>414</v>
+      <c t="s" r="A173">
+        <v>416</v>
       </c>
     </row>
     <row spans="1:1" r="174">
-      <c r="A174" t="s">
-        <v>423</v>
+      <c t="s" r="A174">
+        <v>425</v>
       </c>
     </row>
     <row spans="1:1" r="175">
-      <c r="A175" t="s">
-        <v>424</v>
+      <c t="s" r="A175">
+        <v>426</v>
       </c>
     </row>
     <row spans="1:1" r="176">
-      <c r="A176" t="s">
-        <v>425</v>
+      <c t="s" r="A176">
+        <v>427</v>
       </c>
     </row>
     <row spans="1:1" r="177">
-      <c r="A177" t="s">
-        <v>426</v>
+      <c t="s" r="A177">
+        <v>428</v>
       </c>
     </row>
     <row spans="1:1" r="178">
-      <c r="A178" t="s">
-        <v>436</v>
+      <c t="s" r="A178">
+        <v>438</v>
       </c>
     </row>
     <row spans="1:1" r="179">
-      <c r="A179" t="s">
+      <c t="s" r="A179">
+        <v>441</v>
+      </c>
+    </row>
+    <row spans="1:1" r="180">
+      <c t="s" r="A180">
         <v>439</v>
       </c>
     </row>
-    <row spans="1:1" r="180">
-      <c r="A180" t="s">
-        <v>437</v>
-      </c>
-    </row>
     <row spans="1:1" r="181">
-      <c r="A181" t="s">
+      <c t="s" r="A181">
+        <v>442</v>
+      </c>
+    </row>
+    <row spans="1:1" r="182">
+      <c t="s" r="A182">
         <v>440</v>
       </c>
     </row>
-    <row spans="1:1" r="182">
-      <c r="A182" t="s">
-        <v>438</v>
-      </c>
-    </row>
     <row spans="1:1" r="183">
-      <c r="A183" t="s">
-        <v>448</v>
+      <c t="s" r="A183">
+        <v>450</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins top="1" footer="0.5" right="0.75" header="0.5" left="0.75" bottom="1"/>
+  <pageMargins bottom="1" right="0.75" left="0.75" top="1" footer="0.5" header="0.5"/>
 </worksheet>
 </file>
 
@@ -2824,1271 +2854,1271 @@
   <sheetFormatPr defaultRowHeight="15" baseColWidth="10"/>
   <sheetData>
     <row spans="1:1" r="1">
-      <c r="A1" t="s">
+      <c t="s" r="A1">
         <v>0</v>
       </c>
     </row>
     <row spans="1:1" r="2">
-      <c r="A2" t="s">
+      <c t="s" r="A2">
         <v>1</v>
       </c>
     </row>
     <row spans="1:1" r="3">
-      <c r="A3" t="s">
+      <c t="s" r="A3">
         <v>2</v>
       </c>
     </row>
     <row spans="1:1" r="4">
-      <c r="A4" t="s">
+      <c t="s" r="A4">
         <v>3</v>
       </c>
     </row>
     <row spans="1:1" r="5">
-      <c r="A5" t="s">
+      <c t="s" r="A5">
         <v>4</v>
       </c>
     </row>
     <row spans="1:1" r="6">
-      <c r="A6" t="s">
+      <c t="s" r="A6">
         <v>5</v>
       </c>
     </row>
     <row spans="1:1" r="7">
-      <c r="A7" t="s">
+      <c t="s" r="A7">
         <v>6</v>
       </c>
     </row>
     <row spans="1:1" r="8">
-      <c r="A8" t="s">
+      <c t="s" r="A8">
         <v>7</v>
       </c>
     </row>
     <row spans="1:1" r="9">
-      <c r="A9" t="s">
+      <c t="s" r="A9">
         <v>8</v>
       </c>
     </row>
     <row spans="1:1" r="10">
-      <c r="A10" t="s">
+      <c t="s" r="A10">
         <v>9</v>
       </c>
     </row>
     <row spans="1:1" r="11">
-      <c r="A11" t="s">
+      <c t="s" r="A11">
         <v>10</v>
       </c>
     </row>
     <row spans="1:1" r="12">
-      <c r="A12" t="s">
+      <c t="s" r="A12">
         <v>12</v>
       </c>
     </row>
     <row spans="1:1" r="13">
-      <c r="A13" t="s">
+      <c t="s" r="A13">
         <v>13</v>
       </c>
     </row>
     <row spans="1:1" r="14">
-      <c r="A14" t="s">
+      <c t="s" r="A14">
         <v>14</v>
       </c>
     </row>
     <row spans="1:1" r="15">
-      <c r="A15" t="s">
+      <c t="s" r="A15">
         <v>15</v>
       </c>
     </row>
     <row spans="1:1" r="16">
-      <c r="A16" t="s">
+      <c t="s" r="A16">
         <v>16</v>
       </c>
     </row>
     <row spans="1:1" r="17">
-      <c r="A17" t="s">
+      <c t="s" r="A17">
         <v>69</v>
       </c>
     </row>
     <row spans="1:1" r="18">
-      <c r="A18" t="s">
+      <c t="s" r="A18">
         <v>70</v>
       </c>
     </row>
     <row spans="1:1" r="19">
-      <c r="A19" t="s">
+      <c t="s" r="A19">
         <v>71</v>
       </c>
     </row>
     <row spans="1:1" r="20">
-      <c r="A20" t="s">
+      <c t="s" r="A20">
         <v>72</v>
       </c>
     </row>
     <row spans="1:1" r="21">
-      <c r="A21" t="s">
+      <c t="s" r="A21">
         <v>73</v>
       </c>
     </row>
     <row spans="1:1" r="22">
-      <c r="A22" t="s">
+      <c t="s" r="A22">
         <v>74</v>
       </c>
     </row>
     <row spans="1:1" r="23">
-      <c r="A23" t="s">
+      <c t="s" r="A23">
         <v>75</v>
       </c>
     </row>
     <row spans="1:1" r="24">
-      <c r="A24" t="s">
+      <c t="s" r="A24">
         <v>76</v>
       </c>
     </row>
     <row spans="1:1" r="25">
-      <c r="A25" t="s">
+      <c t="s" r="A25">
         <v>77</v>
       </c>
     </row>
     <row spans="1:1" r="26">
-      <c r="A26" t="s">
+      <c t="s" r="A26">
         <v>78</v>
       </c>
     </row>
     <row spans="1:1" r="27">
-      <c r="A27" t="s">
+      <c t="s" r="A27">
         <v>79</v>
       </c>
     </row>
     <row spans="1:1" r="28">
-      <c r="A28" t="s">
+      <c t="s" r="A28">
         <v>80</v>
       </c>
     </row>
     <row spans="1:1" r="29">
-      <c r="A29" t="s">
+      <c t="s" r="A29">
         <v>81</v>
       </c>
     </row>
     <row spans="1:1" r="30">
-      <c r="A30" t="s">
+      <c t="s" r="A30">
         <v>82</v>
       </c>
     </row>
     <row spans="1:1" r="31">
-      <c r="A31" t="s">
+      <c t="s" r="A31">
         <v>83</v>
       </c>
     </row>
     <row spans="1:1" r="32">
-      <c r="A32" t="s">
+      <c t="s" r="A32">
         <v>84</v>
       </c>
     </row>
     <row spans="1:1" r="33">
-      <c r="A33" t="s">
+      <c t="s" r="A33">
         <v>85</v>
       </c>
     </row>
     <row spans="1:1" r="34">
-      <c r="A34" t="s">
+      <c t="s" r="A34">
         <v>86</v>
       </c>
     </row>
     <row spans="1:1" r="35">
-      <c r="A35" t="s">
+      <c t="s" r="A35">
         <v>87</v>
       </c>
     </row>
     <row spans="1:1" r="36">
-      <c r="A36" t="s">
+      <c t="s" r="A36">
         <v>93</v>
       </c>
     </row>
     <row spans="1:1" r="37">
-      <c r="A37" t="s">
+      <c t="s" r="A37">
         <v>94</v>
       </c>
     </row>
     <row spans="1:1" r="38">
-      <c r="A38" t="s">
+      <c t="s" r="A38">
         <v>95</v>
       </c>
     </row>
     <row spans="1:1" r="39">
-      <c r="A39" t="s">
+      <c t="s" r="A39">
         <v>96</v>
       </c>
     </row>
     <row spans="1:1" r="40">
-      <c r="A40" t="s">
+      <c t="s" r="A40">
         <v>97</v>
       </c>
     </row>
     <row spans="1:1" r="41">
-      <c r="A41" t="s">
+      <c t="s" r="A41">
         <v>98</v>
       </c>
     </row>
     <row spans="1:1" r="42">
-      <c r="A42" t="s">
+      <c t="s" r="A42">
         <v>102</v>
       </c>
     </row>
     <row spans="1:1" r="43">
-      <c r="A43" t="s">
+      <c t="s" r="A43">
         <v>103</v>
       </c>
     </row>
     <row spans="1:1" r="44">
-      <c r="A44" t="s">
+      <c t="s" r="A44">
         <v>104</v>
       </c>
     </row>
     <row spans="1:1" r="45">
-      <c r="A45" t="s">
+      <c t="s" r="A45">
         <v>105</v>
       </c>
     </row>
     <row spans="1:1" r="46">
-      <c r="A46" t="s">
+      <c t="s" r="A46">
         <v>106</v>
       </c>
     </row>
     <row spans="1:1" r="47">
-      <c r="A47" t="s">
+      <c t="s" r="A47">
         <v>108</v>
       </c>
     </row>
     <row spans="1:1" r="48">
-      <c r="A48" t="s">
+      <c t="s" r="A48">
         <v>109</v>
       </c>
     </row>
     <row spans="1:1" r="49">
-      <c r="A49" t="s">
+      <c t="s" r="A49">
         <v>110</v>
       </c>
     </row>
     <row spans="1:1" r="50">
-      <c r="A50" t="s">
+      <c t="s" r="A50">
         <v>111</v>
       </c>
     </row>
     <row spans="1:1" r="51">
-      <c r="A51" t="s">
+      <c t="s" r="A51">
         <v>112</v>
       </c>
     </row>
     <row spans="1:1" r="52">
-      <c r="A52" t="s">
+      <c t="s" r="A52">
         <v>113</v>
       </c>
     </row>
     <row spans="1:1" r="53">
-      <c r="A53" t="s">
+      <c t="s" r="A53">
         <v>114</v>
       </c>
     </row>
     <row spans="1:1" r="54">
-      <c r="A54" t="s">
+      <c t="s" r="A54">
         <v>130</v>
       </c>
     </row>
     <row spans="1:1" r="55">
-      <c r="A55" t="s">
+      <c t="s" r="A55">
         <v>131</v>
       </c>
     </row>
     <row spans="1:1" r="56">
-      <c r="A56" t="s">
+      <c t="s" r="A56">
         <v>132</v>
       </c>
     </row>
     <row spans="1:1" r="57">
-      <c r="A57" t="s">
+      <c t="s" r="A57">
         <v>133</v>
       </c>
     </row>
     <row spans="1:1" r="58">
-      <c r="A58" t="s">
+      <c t="s" r="A58">
         <v>134</v>
       </c>
     </row>
     <row spans="1:1" r="59">
-      <c r="A59" t="s">
+      <c t="s" r="A59">
         <v>135</v>
       </c>
     </row>
     <row spans="1:1" r="60">
-      <c r="A60" t="s">
+      <c t="s" r="A60">
         <v>138</v>
       </c>
     </row>
     <row spans="1:1" r="61">
-      <c r="A61" t="s">
+      <c t="s" r="A61">
         <v>140</v>
       </c>
     </row>
     <row spans="1:1" r="62">
-      <c r="A62" t="s">
+      <c t="s" r="A62">
         <v>141</v>
       </c>
     </row>
     <row spans="1:1" r="63">
-      <c r="A63" t="s">
+      <c t="s" r="A63">
         <v>142</v>
       </c>
     </row>
     <row spans="1:1" r="64">
-      <c r="A64" t="s">
+      <c t="s" r="A64">
         <v>143</v>
       </c>
     </row>
     <row spans="1:1" r="65">
-      <c r="A65" t="s">
+      <c t="s" r="A65">
         <v>144</v>
       </c>
     </row>
     <row spans="1:1" r="66">
-      <c r="A66" t="s">
+      <c t="s" r="A66">
         <v>145</v>
       </c>
     </row>
     <row spans="1:1" r="67">
-      <c r="A67" t="s">
+      <c t="s" r="A67">
         <v>155</v>
       </c>
     </row>
     <row spans="1:1" r="68">
-      <c r="A68" t="s">
+      <c t="s" r="A68">
         <v>156</v>
       </c>
     </row>
     <row spans="1:1" r="69">
-      <c r="A69" t="s">
+      <c t="s" r="A69">
         <v>157</v>
       </c>
     </row>
     <row spans="1:1" r="70">
-      <c r="A70" t="s">
+      <c t="s" r="A70">
         <v>158</v>
       </c>
     </row>
     <row spans="1:1" r="71">
-      <c r="A71" t="s">
+      <c t="s" r="A71">
         <v>159</v>
       </c>
     </row>
     <row spans="1:1" r="72">
-      <c r="A72" t="s">
+      <c t="s" r="A72">
         <v>160</v>
       </c>
     </row>
     <row spans="1:1" r="73">
-      <c r="A73" t="s">
+      <c t="s" r="A73">
         <v>161</v>
       </c>
     </row>
     <row spans="1:1" r="74">
-      <c r="A74" t="s">
+      <c t="s" r="A74">
         <v>165</v>
       </c>
     </row>
     <row spans="1:1" r="75">
-      <c r="A75" t="s">
+      <c t="s" r="A75">
         <v>166</v>
       </c>
     </row>
     <row spans="1:1" r="76">
-      <c r="A76" t="s">
+      <c t="s" r="A76">
         <v>167</v>
       </c>
     </row>
     <row spans="1:1" r="77">
-      <c r="A77" t="s">
+      <c t="s" r="A77">
         <v>168</v>
       </c>
     </row>
     <row spans="1:1" r="78">
-      <c r="A78" t="s">
+      <c t="s" r="A78">
         <v>169</v>
       </c>
     </row>
     <row spans="1:1" r="79">
-      <c r="A79" t="s">
+      <c t="s" r="A79">
         <v>170</v>
       </c>
     </row>
     <row spans="1:1" r="80">
-      <c r="A80" t="s">
+      <c t="s" r="A80">
         <v>171</v>
       </c>
     </row>
     <row spans="1:1" r="81">
-      <c r="A81" t="s">
+      <c t="s" r="A81">
         <v>172</v>
       </c>
     </row>
     <row spans="1:1" r="82">
-      <c r="A82" t="s">
+      <c t="s" r="A82">
         <v>173</v>
       </c>
     </row>
     <row spans="1:1" r="83">
-      <c r="A83" t="s">
+      <c t="s" r="A83">
         <v>174</v>
       </c>
     </row>
     <row spans="1:1" r="84">
-      <c r="A84" t="s">
+      <c t="s" r="A84">
         <v>176</v>
       </c>
     </row>
     <row spans="1:1" r="85">
-      <c r="A85" t="s">
+      <c t="s" r="A85">
         <v>177</v>
       </c>
     </row>
     <row spans="1:1" r="86">
-      <c r="A86" t="s">
+      <c t="s" r="A86">
         <v>178</v>
       </c>
     </row>
     <row spans="1:1" r="87">
-      <c r="A87" t="s">
+      <c t="s" r="A87">
         <v>179</v>
       </c>
     </row>
     <row spans="1:1" r="88">
-      <c r="A88" t="s">
+      <c t="s" r="A88">
         <v>180</v>
       </c>
     </row>
     <row spans="1:1" r="89">
-      <c r="A89" t="s">
+      <c t="s" r="A89">
         <v>181</v>
       </c>
     </row>
     <row spans="1:1" r="90">
-      <c r="A90" t="s">
+      <c t="s" r="A90">
         <v>182</v>
       </c>
     </row>
     <row spans="1:1" r="91">
-      <c r="A91" t="s">
+      <c t="s" r="A91">
         <v>183</v>
       </c>
     </row>
     <row spans="1:1" r="92">
-      <c r="A92" t="s">
+      <c t="s" r="A92">
         <v>191</v>
       </c>
     </row>
     <row spans="1:1" r="93">
-      <c r="A93" t="s">
+      <c t="s" r="A93">
         <v>192</v>
       </c>
     </row>
     <row spans="1:1" r="94">
-      <c r="A94" t="s">
+      <c t="s" r="A94">
         <v>193</v>
       </c>
     </row>
     <row spans="1:1" r="95">
-      <c r="A95" t="s">
+      <c t="s" r="A95">
         <v>194</v>
       </c>
     </row>
     <row spans="1:1" r="96">
-      <c r="A96" t="s">
+      <c t="s" r="A96">
         <v>195</v>
       </c>
     </row>
     <row spans="1:1" r="97">
-      <c r="A97" t="s">
-        <v>196</v>
+      <c t="s" r="A97">
+        <v>197</v>
       </c>
     </row>
     <row spans="1:1" r="98">
-      <c r="A98" t="s">
-        <v>197</v>
+      <c t="s" r="A98">
+        <v>198</v>
       </c>
     </row>
     <row spans="1:1" r="99">
-      <c r="A99" t="s">
-        <v>198</v>
+      <c t="s" r="A99">
+        <v>199</v>
       </c>
     </row>
     <row spans="1:1" r="100">
-      <c r="A100" t="s">
-        <v>199</v>
+      <c t="s" r="A100">
+        <v>200</v>
       </c>
     </row>
     <row spans="1:1" r="101">
-      <c r="A101" t="s">
-        <v>200</v>
+      <c t="s" r="A101">
+        <v>201</v>
       </c>
     </row>
     <row spans="1:1" r="102">
-      <c r="A102" t="s">
+      <c t="s" r="A102">
+        <v>203</v>
+      </c>
+    </row>
+    <row spans="1:1" r="103">
+      <c t="s" r="A103">
+        <v>204</v>
+      </c>
+    </row>
+    <row spans="1:1" r="104">
+      <c t="s" r="A104">
+        <v>205</v>
+      </c>
+    </row>
+    <row spans="1:1" r="105">
+      <c t="s" r="A105">
+        <v>206</v>
+      </c>
+    </row>
+    <row spans="1:1" r="106">
+      <c t="s" r="A106">
+        <v>207</v>
+      </c>
+    </row>
+    <row spans="1:1" r="107">
+      <c t="s" r="A107">
+        <v>225</v>
+      </c>
+    </row>
+    <row spans="1:1" r="108">
+      <c t="s" r="A108">
+        <v>226</v>
+      </c>
+    </row>
+    <row spans="1:1" r="109">
+      <c t="s" r="A109">
+        <v>227</v>
+      </c>
+    </row>
+    <row spans="1:1" r="110">
+      <c t="s" r="A110">
+        <v>228</v>
+      </c>
+    </row>
+    <row spans="1:1" r="111">
+      <c t="s" r="A111">
+        <v>229</v>
+      </c>
+    </row>
+    <row spans="1:1" r="112">
+      <c t="s" r="A112">
+        <v>230</v>
+      </c>
+    </row>
+    <row spans="1:1" r="113">
+      <c t="s" r="A113">
+        <v>231</v>
+      </c>
+    </row>
+    <row spans="1:1" r="114">
+      <c t="s" r="A114">
+        <v>232</v>
+      </c>
+    </row>
+    <row spans="1:1" r="115">
+      <c t="s" r="A115">
+        <v>233</v>
+      </c>
+    </row>
+    <row spans="1:1" r="116">
+      <c t="s" r="A116">
+        <v>234</v>
+      </c>
+    </row>
+    <row spans="1:1" r="117">
+      <c t="s" r="A117">
+        <v>235</v>
+      </c>
+    </row>
+    <row spans="1:1" r="118">
+      <c t="s" r="A118">
+        <v>236</v>
+      </c>
+    </row>
+    <row spans="1:1" r="119">
+      <c t="s" r="A119">
+        <v>237</v>
+      </c>
+    </row>
+    <row spans="1:1" r="120">
+      <c t="s" r="A120">
+        <v>238</v>
+      </c>
+    </row>
+    <row spans="1:1" r="121">
+      <c t="s" r="A121">
+        <v>242</v>
+      </c>
+    </row>
+    <row spans="1:1" r="122">
+      <c t="s" r="A122">
+        <v>243</v>
+      </c>
+    </row>
+    <row spans="1:1" r="123">
+      <c t="s" r="A123">
+        <v>244</v>
+      </c>
+    </row>
+    <row spans="1:1" r="124">
+      <c t="s" r="A124">
+        <v>245</v>
+      </c>
+    </row>
+    <row spans="1:1" r="125">
+      <c t="s" r="A125">
+        <v>246</v>
+      </c>
+    </row>
+    <row spans="1:1" r="126">
+      <c t="s" r="A126">
+        <v>247</v>
+      </c>
+    </row>
+    <row spans="1:1" r="127">
+      <c t="s" r="A127">
+        <v>248</v>
+      </c>
+    </row>
+    <row spans="1:1" r="128">
+      <c t="s" r="A128">
+        <v>249</v>
+      </c>
+    </row>
+    <row spans="1:1" r="129">
+      <c t="s" r="A129">
+        <v>250</v>
+      </c>
+    </row>
+    <row spans="1:1" r="130">
+      <c t="s" r="A130">
+        <v>251</v>
+      </c>
+    </row>
+    <row spans="1:1" r="131">
+      <c t="s" r="A131">
+        <v>252</v>
+      </c>
+    </row>
+    <row spans="1:1" r="132">
+      <c t="s" r="A132">
+        <v>257</v>
+      </c>
+    </row>
+    <row spans="1:1" r="133">
+      <c t="s" r="A133">
+        <v>258</v>
+      </c>
+    </row>
+    <row spans="1:1" r="134">
+      <c t="s" r="A134">
+        <v>259</v>
+      </c>
+    </row>
+    <row spans="1:1" r="135">
+      <c t="s" r="A135">
+        <v>260</v>
+      </c>
+    </row>
+    <row spans="1:1" r="136">
+      <c t="s" r="A136">
+        <v>261</v>
+      </c>
+    </row>
+    <row spans="1:1" r="137">
+      <c t="s" r="A137">
+        <v>263</v>
+      </c>
+    </row>
+    <row spans="1:1" r="138">
+      <c t="s" r="A138">
+        <v>264</v>
+      </c>
+    </row>
+    <row spans="1:1" r="139">
+      <c t="s" r="A139">
+        <v>265</v>
+      </c>
+    </row>
+    <row spans="1:1" r="140">
+      <c t="s" r="A140">
+        <v>266</v>
+      </c>
+    </row>
+    <row spans="1:1" r="141">
+      <c t="s" r="A141">
+        <v>267</v>
+      </c>
+    </row>
+    <row spans="1:1" r="142">
+      <c t="s" r="A142">
+        <v>268</v>
+      </c>
+    </row>
+    <row spans="1:1" r="143">
+      <c t="s" r="A143">
+        <v>269</v>
+      </c>
+    </row>
+    <row spans="1:1" r="144">
+      <c t="s" r="A144">
+        <v>270</v>
+      </c>
+    </row>
+    <row spans="1:1" r="145">
+      <c t="s" r="A145">
+        <v>271</v>
+      </c>
+    </row>
+    <row spans="1:1" r="146">
+      <c t="s" r="A146">
+        <v>272</v>
+      </c>
+    </row>
+    <row spans="1:1" r="147">
+      <c t="s" r="A147">
+        <v>273</v>
+      </c>
+    </row>
+    <row spans="1:1" r="148">
+      <c t="s" r="A148">
+        <v>274</v>
+      </c>
+    </row>
+    <row spans="1:1" r="149">
+      <c t="s" r="A149">
+        <v>275</v>
+      </c>
+    </row>
+    <row spans="1:1" r="150">
+      <c t="s" r="A150">
+        <v>276</v>
+      </c>
+    </row>
+    <row spans="1:1" r="151">
+      <c t="s" r="A151">
+        <v>277</v>
+      </c>
+    </row>
+    <row spans="1:1" r="152">
+      <c t="s" r="A152">
+        <v>278</v>
+      </c>
+    </row>
+    <row spans="1:1" r="153">
+      <c t="s" r="A153">
+        <v>280</v>
+      </c>
+    </row>
+    <row spans="1:1" r="154">
+      <c t="s" r="A154">
+        <v>282</v>
+      </c>
+    </row>
+    <row spans="1:1" r="155">
+      <c t="s" r="A155">
+        <v>283</v>
+      </c>
+    </row>
+    <row spans="1:1" r="156">
+      <c t="s" r="A156">
+        <v>285</v>
+      </c>
+    </row>
+    <row spans="1:1" r="157">
+      <c t="s" r="A157">
+        <v>286</v>
+      </c>
+    </row>
+    <row spans="1:1" r="158">
+      <c t="s" r="A158">
+        <v>287</v>
+      </c>
+    </row>
+    <row spans="1:1" r="159">
+      <c t="s" r="A159">
+        <v>288</v>
+      </c>
+    </row>
+    <row spans="1:1" r="160">
+      <c t="s" r="A160">
+        <v>289</v>
+      </c>
+    </row>
+    <row spans="1:1" r="161">
+      <c t="s" r="A161">
+        <v>290</v>
+      </c>
+    </row>
+    <row spans="1:1" r="162">
+      <c t="s" r="A162">
+        <v>291</v>
+      </c>
+    </row>
+    <row spans="1:1" r="163">
+      <c t="s" r="A163">
+        <v>292</v>
+      </c>
+    </row>
+    <row spans="1:1" r="164">
+      <c t="s" r="A164">
+        <v>293</v>
+      </c>
+    </row>
+    <row spans="1:1" r="165">
+      <c t="s" r="A165">
+        <v>294</v>
+      </c>
+    </row>
+    <row spans="1:1" r="166">
+      <c t="s" r="A166">
+        <v>318</v>
+      </c>
+    </row>
+    <row spans="1:1" r="167">
+      <c t="s" r="A167">
+        <v>323</v>
+      </c>
+    </row>
+    <row spans="1:1" r="168">
+      <c t="s" r="A168">
+        <v>324</v>
+      </c>
+    </row>
+    <row spans="1:1" r="169">
+      <c t="s" r="A169">
+        <v>325</v>
+      </c>
+    </row>
+    <row spans="1:1" r="170">
+      <c t="s" r="A170">
+        <v>326</v>
+      </c>
+    </row>
+    <row spans="1:1" r="171">
+      <c t="s" r="A171">
+        <v>327</v>
+      </c>
+    </row>
+    <row spans="1:1" r="172">
+      <c t="s" r="A172">
+        <v>328</v>
+      </c>
+    </row>
+    <row spans="1:1" r="173">
+      <c t="s" r="A173">
+        <v>329</v>
+      </c>
+    </row>
+    <row spans="1:1" r="174">
+      <c t="s" r="A174">
+        <v>330</v>
+      </c>
+    </row>
+    <row spans="1:1" r="175">
+      <c t="s" r="A175">
+        <v>331</v>
+      </c>
+    </row>
+    <row spans="1:1" r="176">
+      <c t="s" r="A176">
+        <v>332</v>
+      </c>
+    </row>
+    <row spans="1:1" r="177">
+      <c t="s" r="A177">
+        <v>333</v>
+      </c>
+    </row>
+    <row spans="1:1" r="178">
+      <c t="s" r="A178">
+        <v>334</v>
+      </c>
+    </row>
+    <row spans="1:1" r="179">
+      <c t="s" r="A179">
+        <v>335</v>
+      </c>
+    </row>
+    <row spans="1:1" r="180">
+      <c t="s" r="A180">
+        <v>340</v>
+      </c>
+    </row>
+    <row spans="1:1" r="181">
+      <c t="s" r="A181">
+        <v>341</v>
+      </c>
+    </row>
+    <row spans="1:1" r="182">
+      <c t="s" r="A182">
+        <v>342</v>
+      </c>
+    </row>
+    <row spans="1:1" r="183">
+      <c t="s" r="A183">
+        <v>343</v>
+      </c>
+    </row>
+    <row spans="1:1" r="184">
+      <c t="s" r="A184">
+        <v>344</v>
+      </c>
+    </row>
+    <row spans="1:1" r="185">
+      <c t="s" r="A185">
+        <v>361</v>
+      </c>
+    </row>
+    <row spans="1:1" r="186">
+      <c t="s" r="A186">
+        <v>381</v>
+      </c>
+    </row>
+    <row spans="1:1" r="187">
+      <c t="s" r="A187">
+        <v>362</v>
+      </c>
+    </row>
+    <row spans="1:1" r="188">
+      <c t="s" r="A188">
+        <v>363</v>
+      </c>
+    </row>
+    <row spans="1:1" r="189">
+      <c t="s" r="A189">
+        <v>364</v>
+      </c>
+    </row>
+    <row spans="1:1" r="190">
+      <c t="s" r="A190">
+        <v>365</v>
+      </c>
+    </row>
+    <row spans="1:1" r="191">
+      <c t="s" r="A191">
+        <v>366</v>
+      </c>
+    </row>
+    <row spans="1:1" r="192">
+      <c t="s" r="A192">
+        <v>367</v>
+      </c>
+    </row>
+    <row spans="1:1" r="193">
+      <c t="s" r="A193">
+        <v>368</v>
+      </c>
+    </row>
+    <row spans="1:1" r="194">
+      <c t="s" r="A194">
+        <v>369</v>
+      </c>
+    </row>
+    <row spans="1:1" r="195">
+      <c t="s" r="A195">
+        <v>370</v>
+      </c>
+    </row>
+    <row spans="1:1" r="196">
+      <c t="s" r="A196">
+        <v>371</v>
+      </c>
+    </row>
+    <row spans="1:1" r="197">
+      <c t="s" r="A197">
+        <v>372</v>
+      </c>
+    </row>
+    <row spans="1:1" r="198">
+      <c t="s" r="A198">
+        <v>373</v>
+      </c>
+    </row>
+    <row spans="1:1" r="199">
+      <c t="s" r="A199">
+        <v>374</v>
+      </c>
+    </row>
+    <row spans="1:1" r="200">
+      <c t="s" r="A200">
+        <v>375</v>
+      </c>
+    </row>
+    <row spans="1:1" r="201">
+      <c t="s" r="A201">
+        <v>376</v>
+      </c>
+    </row>
+    <row spans="1:1" r="202">
+      <c t="s" r="A202">
+        <v>377</v>
+      </c>
+    </row>
+    <row spans="1:1" r="203">
+      <c t="s" r="A203">
+        <v>378</v>
+      </c>
+    </row>
+    <row spans="1:1" r="204">
+      <c t="s" r="A204">
+        <v>379</v>
+      </c>
+    </row>
+    <row spans="1:1" r="205">
+      <c t="s" r="A205">
+        <v>396</v>
+      </c>
+    </row>
+    <row spans="1:1" r="206">
+      <c t="s" r="A206">
+        <v>397</v>
+      </c>
+    </row>
+    <row spans="1:1" r="207">
+      <c t="s" r="A207">
+        <v>398</v>
+      </c>
+    </row>
+    <row spans="1:1" r="208">
+      <c t="s" r="A208">
+        <v>399</v>
+      </c>
+    </row>
+    <row spans="1:1" r="209">
+      <c t="s" r="A209">
+        <v>400</v>
+      </c>
+    </row>
+    <row spans="1:1" r="210">
+      <c t="s" r="A210">
+        <v>401</v>
+      </c>
+    </row>
+    <row spans="1:1" r="211">
+      <c t="s" r="A211">
+        <v>402</v>
+      </c>
+    </row>
+    <row spans="1:1" r="212">
+      <c t="s" r="A212">
+        <v>404</v>
+      </c>
+    </row>
+    <row spans="1:1" r="213">
+      <c t="s" r="A213">
+        <v>405</v>
+      </c>
+    </row>
+    <row spans="1:1" r="214">
+      <c t="s" r="A214">
+        <v>406</v>
+      </c>
+    </row>
+    <row spans="1:1" r="215">
+      <c t="s" r="A215">
+        <v>407</v>
+      </c>
+    </row>
+    <row spans="1:1" r="216">
+      <c t="s" r="A216">
+        <v>408</v>
+      </c>
+    </row>
+    <row spans="1:1" r="217">
+      <c t="s" r="A217">
+        <v>409</v>
+      </c>
+    </row>
+    <row spans="1:1" r="218">
+      <c t="s" r="A218">
+        <v>410</v>
+      </c>
+    </row>
+    <row spans="1:1" r="219">
+      <c t="s" r="A219">
+        <v>411</v>
+      </c>
+    </row>
+    <row spans="1:1" r="220">
+      <c t="s" r="A220">
+        <v>412</v>
+      </c>
+    </row>
+    <row spans="1:1" r="221">
+      <c t="s" r="A221">
+        <v>417</v>
+      </c>
+    </row>
+    <row spans="1:1" r="222">
+      <c t="s" r="A222">
+        <v>418</v>
+      </c>
+    </row>
+    <row spans="1:1" r="223">
+      <c t="s" r="A223">
+        <v>419</v>
+      </c>
+    </row>
+    <row spans="1:1" r="224">
+      <c t="s" r="A224">
+        <v>420</v>
+      </c>
+    </row>
+    <row spans="1:1" r="225">
+      <c t="s" r="A225">
+        <v>422</v>
+      </c>
+    </row>
+    <row spans="1:1" r="226">
+      <c t="s" r="A226">
+        <v>423</v>
+      </c>
+    </row>
+    <row spans="1:1" r="227">
+      <c t="s" r="A227">
+        <v>424</v>
+      </c>
+    </row>
+    <row spans="1:1" r="228">
+      <c t="s" r="A228">
+        <v>429</v>
+      </c>
+    </row>
+    <row spans="1:1" r="229">
+      <c t="s" r="A229">
+        <v>430</v>
+      </c>
+    </row>
+    <row spans="1:1" r="230">
+      <c t="s" r="A230">
+        <v>431</v>
+      </c>
+    </row>
+    <row spans="1:1" r="231">
+      <c t="s" r="A231">
+        <v>432</v>
+      </c>
+    </row>
+    <row spans="1:1" r="232">
+      <c t="s" r="A232">
+        <v>433</v>
+      </c>
+    </row>
+    <row spans="1:1" r="233">
+      <c t="s" r="A233">
+        <v>434</v>
+      </c>
+    </row>
+    <row spans="1:1" r="234">
+      <c t="s" r="A234">
+        <v>435</v>
+      </c>
+    </row>
+    <row spans="1:1" r="235">
+      <c t="s" r="A235">
+        <v>436</v>
+      </c>
+    </row>
+    <row spans="1:1" r="236">
+      <c t="s" r="A236">
+        <v>437</v>
+      </c>
+    </row>
+    <row spans="1:1" r="237">
+      <c t="s" r="A237">
+        <v>443</v>
+      </c>
+    </row>
+    <row spans="1:1" r="238">
+      <c t="s" r="A238">
+        <v>444</v>
+      </c>
+    </row>
+    <row spans="1:1" r="239">
+      <c t="s" r="A239">
+        <v>445</v>
+      </c>
+    </row>
+    <row spans="1:1" r="240">
+      <c t="s" r="A240">
+        <v>446</v>
+      </c>
+    </row>
+    <row spans="1:1" r="241">
+      <c t="s" r="A241">
+        <v>447</v>
+      </c>
+    </row>
+    <row spans="1:1" r="242">
+      <c t="s" r="A242">
+        <v>448</v>
+      </c>
+    </row>
+    <row spans="1:1" r="243">
+      <c t="s" r="A243">
+        <v>449</v>
+      </c>
+    </row>
+    <row spans="1:1" r="244">
+      <c t="s" r="A244">
+        <v>107</v>
+      </c>
+    </row>
+    <row spans="1:1" r="245">
+      <c t="s" r="A245">
+        <v>139</v>
+      </c>
+    </row>
+    <row spans="1:1" r="246">
+      <c t="s" r="A246">
+        <v>175</v>
+      </c>
+    </row>
+    <row spans="1:1" r="247">
+      <c t="s" r="A247">
         <v>202</v>
       </c>
     </row>
-    <row spans="1:1" r="103">
-      <c r="A103" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row spans="1:1" r="104">
-      <c r="A104" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row spans="1:1" r="105">
-      <c r="A105" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row spans="1:1" r="106">
-      <c r="A106" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row spans="1:1" r="107">
-      <c r="A107" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row spans="1:1" r="108">
-      <c r="A108" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row spans="1:1" r="109">
-      <c r="A109" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row spans="1:1" r="110">
-      <c r="A110" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row spans="1:1" r="111">
-      <c r="A111" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row spans="1:1" r="112">
-      <c r="A112" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row spans="1:1" r="113">
-      <c r="A113" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row spans="1:1" r="114">
-      <c r="A114" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row spans="1:1" r="115">
-      <c r="A115" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row spans="1:1" r="116">
-      <c r="A116" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row spans="1:1" r="117">
-      <c r="A117" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row spans="1:1" r="118">
-      <c r="A118" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row spans="1:1" r="119">
-      <c r="A119" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row spans="1:1" r="120">
-      <c r="A120" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row spans="1:1" r="121">
-      <c r="A121" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row spans="1:1" r="122">
-      <c r="A122" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row spans="1:1" r="123">
-      <c r="A123" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row spans="1:1" r="124">
-      <c r="A124" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row spans="1:1" r="125">
-      <c r="A125" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row spans="1:1" r="126">
-      <c r="A126" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row spans="1:1" r="127">
-      <c r="A127" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row spans="1:1" r="128">
-      <c r="A128" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row spans="1:1" r="129">
-      <c r="A129" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row spans="1:1" r="130">
-      <c r="A130" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row spans="1:1" r="131">
-      <c r="A131" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row spans="1:1" r="132">
-      <c r="A132" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row spans="1:1" r="133">
-      <c r="A133" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row spans="1:1" r="134">
-      <c r="A134" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row spans="1:1" r="135">
-      <c r="A135" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row spans="1:1" r="136">
-      <c r="A136" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row spans="1:1" r="137">
-      <c r="A137" t="s">
+    <row spans="1:1" r="248">
+      <c t="s" r="A248">
         <v>262</v>
       </c>
     </row>
-    <row spans="1:1" r="138">
-      <c r="A138" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row spans="1:1" r="139">
-      <c r="A139" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row spans="1:1" r="140">
-      <c r="A140" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row spans="1:1" r="141">
-      <c r="A141" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row spans="1:1" r="142">
-      <c r="A142" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row spans="1:1" r="143">
-      <c r="A143" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row spans="1:1" r="144">
-      <c r="A144" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row spans="1:1" r="145">
-      <c r="A145" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row spans="1:1" r="146">
-      <c r="A146" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row spans="1:1" r="147">
-      <c r="A147" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row spans="1:1" r="148">
-      <c r="A148" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row spans="1:1" r="149">
-      <c r="A149" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row spans="1:1" r="150">
-      <c r="A150" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row spans="1:1" r="151">
-      <c r="A151" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row spans="1:1" r="152">
-      <c r="A152" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row spans="1:1" r="153">
-      <c r="A153" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row spans="1:1" r="154">
-      <c r="A154" t="s">
+    <row spans="1:1" r="249">
+      <c t="s" r="A249">
+        <v>284</v>
+      </c>
+    </row>
+    <row spans="1:1" r="250">
+      <c t="s" r="A250">
+        <v>319</v>
+      </c>
+    </row>
+    <row spans="1:1" r="251">
+      <c t="s" r="A251">
+        <v>11</v>
+      </c>
+    </row>
+    <row spans="1:1" r="252">
+      <c t="s" r="A252">
         <v>281</v>
       </c>
     </row>
-    <row spans="1:1" r="155">
-      <c r="A155" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row spans="1:1" r="156">
-      <c r="A156" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row spans="1:1" r="157">
-      <c r="A157" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row spans="1:1" r="158">
-      <c r="A158" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row spans="1:1" r="159">
-      <c r="A159" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row spans="1:1" r="160">
-      <c r="A160" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row spans="1:1" r="161">
-      <c r="A161" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row spans="1:1" r="162">
-      <c r="A162" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row spans="1:1" r="163">
-      <c r="A163" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row spans="1:1" r="164">
-      <c r="A164" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row spans="1:1" r="165">
-      <c r="A165" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row spans="1:1" r="166">
-      <c r="A166" t="s">
-        <v>316</v>
-      </c>
-    </row>
-    <row spans="1:1" r="167">
-      <c r="A167" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row spans="1:1" r="168">
-      <c r="A168" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row spans="1:1" r="169">
-      <c r="A169" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row spans="1:1" r="170">
-      <c r="A170" t="s">
-        <v>324</v>
-      </c>
-    </row>
-    <row spans="1:1" r="171">
-      <c r="A171" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row spans="1:1" r="172">
-      <c r="A172" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row spans="1:1" r="173">
-      <c r="A173" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row spans="1:1" r="174">
-      <c r="A174" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row spans="1:1" r="175">
-      <c r="A175" t="s">
-        <v>329</v>
-      </c>
-    </row>
-    <row spans="1:1" r="176">
-      <c r="A176" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row spans="1:1" r="177">
-      <c r="A177" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row spans="1:1" r="178">
-      <c r="A178" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row spans="1:1" r="179">
-      <c r="A179" t="s">
-        <v>333</v>
-      </c>
-    </row>
-    <row spans="1:1" r="180">
-      <c r="A180" t="s">
-        <v>338</v>
-      </c>
-    </row>
-    <row spans="1:1" r="181">
-      <c r="A181" t="s">
-        <v>339</v>
-      </c>
-    </row>
-    <row spans="1:1" r="182">
-      <c r="A182" t="s">
-        <v>340</v>
-      </c>
-    </row>
-    <row spans="1:1" r="183">
-      <c r="A183" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row spans="1:1" r="184">
-      <c r="A184" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row spans="1:1" r="185">
-      <c r="A185" t="s">
-        <v>359</v>
-      </c>
-    </row>
-    <row spans="1:1" r="186">
-      <c r="A186" t="s">
-        <v>379</v>
-      </c>
-    </row>
-    <row spans="1:1" r="187">
-      <c r="A187" t="s">
-        <v>360</v>
-      </c>
-    </row>
-    <row spans="1:1" r="188">
-      <c r="A188" t="s">
-        <v>361</v>
-      </c>
-    </row>
-    <row spans="1:1" r="189">
-      <c r="A189" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row spans="1:1" r="190">
-      <c r="A190" t="s">
-        <v>363</v>
-      </c>
-    </row>
-    <row spans="1:1" r="191">
-      <c r="A191" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row spans="1:1" r="192">
-      <c r="A192" t="s">
-        <v>365</v>
-      </c>
-    </row>
-    <row spans="1:1" r="193">
-      <c r="A193" t="s">
-        <v>366</v>
-      </c>
-    </row>
-    <row spans="1:1" r="194">
-      <c r="A194" t="s">
-        <v>367</v>
-      </c>
-    </row>
-    <row spans="1:1" r="195">
-      <c r="A195" t="s">
-        <v>368</v>
-      </c>
-    </row>
-    <row spans="1:1" r="196">
-      <c r="A196" t="s">
-        <v>369</v>
-      </c>
-    </row>
-    <row spans="1:1" r="197">
-      <c r="A197" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row spans="1:1" r="198">
-      <c r="A198" t="s">
-        <v>371</v>
-      </c>
-    </row>
-    <row spans="1:1" r="199">
-      <c r="A199" t="s">
-        <v>372</v>
-      </c>
-    </row>
-    <row spans="1:1" r="200">
-      <c r="A200" t="s">
-        <v>373</v>
-      </c>
-    </row>
-    <row spans="1:1" r="201">
-      <c r="A201" t="s">
-        <v>374</v>
-      </c>
-    </row>
-    <row spans="1:1" r="202">
-      <c r="A202" t="s">
-        <v>375</v>
-      </c>
-    </row>
-    <row spans="1:1" r="203">
-      <c r="A203" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row spans="1:1" r="204">
-      <c r="A204" t="s">
-        <v>377</v>
-      </c>
-    </row>
-    <row spans="1:1" r="205">
-      <c r="A205" t="s">
-        <v>394</v>
-      </c>
-    </row>
-    <row spans="1:1" r="206">
-      <c r="A206" t="s">
-        <v>395</v>
-      </c>
-    </row>
-    <row spans="1:1" r="207">
-      <c r="A207" t="s">
-        <v>396</v>
-      </c>
-    </row>
-    <row spans="1:1" r="208">
-      <c r="A208" t="s">
-        <v>397</v>
-      </c>
-    </row>
-    <row spans="1:1" r="209">
-      <c r="A209" t="s">
-        <v>398</v>
-      </c>
-    </row>
-    <row spans="1:1" r="210">
-      <c r="A210" t="s">
-        <v>399</v>
-      </c>
-    </row>
-    <row spans="1:1" r="211">
-      <c r="A211" t="s">
-        <v>400</v>
-      </c>
-    </row>
-    <row spans="1:1" r="212">
-      <c r="A212" t="s">
-        <v>402</v>
-      </c>
-    </row>
-    <row spans="1:1" r="213">
-      <c r="A213" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row spans="1:1" r="214">
-      <c r="A214" t="s">
-        <v>404</v>
-      </c>
-    </row>
-    <row spans="1:1" r="215">
-      <c r="A215" t="s">
-        <v>405</v>
-      </c>
-    </row>
-    <row spans="1:1" r="216">
-      <c r="A216" t="s">
-        <v>406</v>
-      </c>
-    </row>
-    <row spans="1:1" r="217">
-      <c r="A217" t="s">
-        <v>407</v>
-      </c>
-    </row>
-    <row spans="1:1" r="218">
-      <c r="A218" t="s">
-        <v>408</v>
-      </c>
-    </row>
-    <row spans="1:1" r="219">
-      <c r="A219" t="s">
-        <v>409</v>
-      </c>
-    </row>
-    <row spans="1:1" r="220">
-      <c r="A220" t="s">
-        <v>410</v>
-      </c>
-    </row>
-    <row spans="1:1" r="221">
-      <c r="A221" t="s">
-        <v>415</v>
-      </c>
-    </row>
-    <row spans="1:1" r="222">
-      <c r="A222" t="s">
-        <v>416</v>
-      </c>
-    </row>
-    <row spans="1:1" r="223">
-      <c r="A223" t="s">
-        <v>417</v>
-      </c>
-    </row>
-    <row spans="1:1" r="224">
-      <c r="A224" t="s">
-        <v>418</v>
-      </c>
-    </row>
-    <row spans="1:1" r="225">
-      <c r="A225" t="s">
-        <v>420</v>
-      </c>
-    </row>
-    <row spans="1:1" r="226">
-      <c r="A226" t="s">
-        <v>421</v>
-      </c>
-    </row>
-    <row spans="1:1" r="227">
-      <c r="A227" t="s">
-        <v>422</v>
-      </c>
-    </row>
-    <row spans="1:1" r="228">
-      <c r="A228" t="s">
-        <v>427</v>
-      </c>
-    </row>
-    <row spans="1:1" r="229">
-      <c r="A229" t="s">
-        <v>428</v>
-      </c>
-    </row>
-    <row spans="1:1" r="230">
-      <c r="A230" t="s">
-        <v>429</v>
-      </c>
-    </row>
-    <row spans="1:1" r="231">
-      <c r="A231" t="s">
-        <v>430</v>
-      </c>
-    </row>
-    <row spans="1:1" r="232">
-      <c r="A232" t="s">
-        <v>431</v>
-      </c>
-    </row>
-    <row spans="1:1" r="233">
-      <c r="A233" t="s">
-        <v>432</v>
-      </c>
-    </row>
-    <row spans="1:1" r="234">
-      <c r="A234" t="s">
-        <v>433</v>
-      </c>
-    </row>
-    <row spans="1:1" r="235">
-      <c r="A235" t="s">
-        <v>434</v>
-      </c>
-    </row>
-    <row spans="1:1" r="236">
-      <c r="A236" t="s">
-        <v>435</v>
-      </c>
-    </row>
-    <row spans="1:1" r="237">
-      <c r="A237" t="s">
-        <v>441</v>
-      </c>
-    </row>
-    <row spans="1:1" r="238">
-      <c r="A238" t="s">
-        <v>442</v>
-      </c>
-    </row>
-    <row spans="1:1" r="239">
-      <c r="A239" t="s">
-        <v>443</v>
-      </c>
-    </row>
-    <row spans="1:1" r="240">
-      <c r="A240" t="s">
-        <v>444</v>
-      </c>
-    </row>
-    <row spans="1:1" r="241">
-      <c r="A241" t="s">
-        <v>445</v>
-      </c>
-    </row>
-    <row spans="1:1" r="242">
-      <c r="A242" t="s">
-        <v>446</v>
-      </c>
-    </row>
-    <row spans="1:1" r="243">
-      <c r="A243" t="s">
-        <v>447</v>
-      </c>
-    </row>
-    <row spans="1:1" r="244">
-      <c r="A244" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row spans="1:1" r="245">
-      <c r="A245" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row spans="1:1" r="246">
-      <c r="A246" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row spans="1:1" r="247">
-      <c r="A247" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row spans="1:1" r="248">
-      <c r="A248" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row spans="1:1" r="249">
-      <c r="A249" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row spans="1:1" r="250">
-      <c r="A250" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row spans="1:1" r="251">
-      <c r="A251" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row spans="1:1" r="252">
-      <c r="A252" t="s">
-        <v>280</v>
-      </c>
-    </row>
     <row spans="1:1" r="253">
-      <c r="A253" t="s">
+      <c t="s" r="A253">
         <v>146</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins top="1" footer="0.5" right="0.75" header="0.5" left="0.75" bottom="1"/>
+  <pageMargins bottom="1" right="0.75" left="0.75" top="1" footer="0.5" header="0.5"/>
 </worksheet>
 </file>
</xml_diff>